<commit_message>
[add] excel basic using openpyxl
</commit_message>
<xml_diff>
--- a/RPA-python/sample.xlsx
+++ b/RPA-python/sample.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="jonginSheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,30 +422,132 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D1" t="n">
-        <v>6</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>번호</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>영어</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>수학</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>77</v>
+      </c>
+      <c r="C2" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>98</v>
+      </c>
+      <c r="C3" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="10"/>
+      <c r="B4" t="n">
+        <v>14</v>
+      </c>
+      <c r="C4" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>46</v>
+      </c>
+      <c r="C6" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>14</v>
+      </c>
+      <c r="C7" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>11</v>
+      </c>
+      <c r="C8" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>89</v>
+      </c>
+      <c r="C9" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>63</v>
+      </c>
+      <c r="C11" t="n">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>